<commit_message>
various data bits for usmr dapr3
</commit_message>
<xml_diff>
--- a/basketballhrv.xlsx
+++ b/basketballhrv.xlsx
@@ -97,6 +97,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,20 +182,20 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="167" zoomScaleNormal="167" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="6" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.71"/>
   </cols>
   <sheetData>
@@ -477,9 +478,6 @@
       <c r="F5" s="0" t="n">
         <v>6.45623550111794</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>3.87050115285651</v>
-      </c>
       <c r="H5" s="0" t="n">
         <v>5.13528754850975</v>
       </c>
@@ -592,9 +590,6 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>3.53051473876135</v>
-      </c>
       <c r="C7" s="0" t="n">
         <v>2.88736371865104</v>
       </c>
@@ -645,9 +640,6 @@
       </c>
       <c r="S7" s="0" t="n">
         <v>3.9213973898363</v>
-      </c>
-      <c r="T7" s="0" t="n">
-        <v>4.23744651523503</v>
       </c>
       <c r="U7" s="0" t="n">
         <v>2.5619177849701</v>
@@ -660,9 +652,6 @@
       <c r="B8" s="0" t="n">
         <v>4.76240520352923</v>
       </c>
-      <c r="C8" s="0" t="n">
-        <v>4.57099519206026</v>
-      </c>
       <c r="D8" s="0" t="n">
         <v>3.37328484437645</v>
       </c>
@@ -692,9 +681,6 @@
       </c>
       <c r="M8" s="0" t="n">
         <v>4.11634589457145</v>
-      </c>
-      <c r="N8" s="0" t="n">
-        <v>2.54649152985469</v>
       </c>
       <c r="O8" s="0" t="n">
         <v>4.9880064829376</v>
@@ -817,9 +803,6 @@
       <c r="K10" s="0" t="n">
         <v>4.35333226683034</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <v>1.49056856458689</v>
-      </c>
       <c r="M10" s="0" t="n">
         <v>5.32541122425518</v>
       </c>
@@ -864,9 +847,6 @@
       <c r="E11" s="0" t="n">
         <v>3.93635851000356</v>
       </c>
-      <c r="F11" s="0" t="n">
-        <v>6.09006356883768</v>
-      </c>
       <c r="G11" s="0" t="n">
         <v>4.56403643231994</v>
       </c>
@@ -959,9 +939,6 @@
       <c r="O12" s="0" t="n">
         <v>4.34189987031247</v>
       </c>
-      <c r="P12" s="0" t="n">
-        <v>3.2952345795931</v>
-      </c>
       <c r="Q12" s="0" t="n">
         <v>3.96791049049343</v>
       </c>
@@ -1003,9 +980,6 @@
       <c r="H13" s="0" t="n">
         <v>2.43414343053754</v>
       </c>
-      <c r="I13" s="0" t="n">
-        <v>1.0165796622792</v>
-      </c>
       <c r="J13" s="0" t="n">
         <v>1.69162849948724</v>
       </c>
@@ -1065,9 +1039,6 @@
       <c r="G14" s="0" t="n">
         <v>4.90620345417692</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <v>6.20638939474032</v>
-      </c>
       <c r="I14" s="0" t="n">
         <v>6.48699772428273</v>
       </c>
@@ -1183,14 +1154,8 @@
       <c r="C16" s="0" t="n">
         <v>3.68258291134591</v>
       </c>
-      <c r="D16" s="0" t="n">
-        <v>6.87066790078396</v>
-      </c>
       <c r="E16" s="0" t="n">
         <v>4.43356851635093</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>5.30450162593915</v>
       </c>
       <c r="G16" s="0" t="n">
         <v>6.3742375939756</v>
@@ -1346,9 +1311,6 @@
       <c r="N18" s="0" t="n">
         <v>5.70990882548227</v>
       </c>
-      <c r="O18" s="0" t="n">
-        <v>4.96080298201622</v>
-      </c>
       <c r="P18" s="0" t="n">
         <v>5.05299258459922</v>
       </c>
@@ -1429,9 +1391,6 @@
       <c r="T19" s="0" t="n">
         <v>4.70577845953765</v>
       </c>
-      <c r="U19" s="0" t="n">
-        <v>5.2531438115912</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1556,9 +1515,6 @@
       <c r="S21" s="0" t="n">
         <v>7.15938047262923</v>
       </c>
-      <c r="T21" s="0" t="n">
-        <v>8.17825513909385</v>
-      </c>
       <c r="U21" s="0" t="n">
         <v>4.97798393259853</v>
       </c>
@@ -1573,9 +1529,6 @@
       <c r="C22" s="0" t="n">
         <v>5.56083742518741</v>
       </c>
-      <c r="D22" s="0" t="n">
-        <v>4.34959218121289</v>
-      </c>
       <c r="E22" s="0" t="n">
         <v>4.94297408827765</v>
       </c>
@@ -1599,9 +1552,6 @@
       </c>
       <c r="L22" s="0" t="n">
         <v>5.64012783615762</v>
-      </c>
-      <c r="M22" s="0" t="n">
-        <v>5.80045914326985</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>6.41202274081728</v>
@@ -1647,9 +1597,6 @@
       <c r="F23" s="0" t="n">
         <v>3.36528345343319</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>4.30122974255911</v>
-      </c>
       <c r="H23" s="0" t="n">
         <v>4.74775060359641</v>
       </c>
@@ -1658,9 +1605,6 @@
       </c>
       <c r="J23" s="0" t="n">
         <v>4.10933143901935</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>4.10050750856656</v>
       </c>
       <c r="L23" s="0" t="n">
         <v>4.74614545728319</v>
@@ -1715,9 +1659,6 @@
       <c r="G24" s="0" t="n">
         <v>5.67375506683509</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <v>4.56784281968635</v>
-      </c>
       <c r="I24" s="0" t="n">
         <v>5.41668164515419</v>
       </c>
@@ -1949,9 +1890,6 @@
       <c r="T27" s="0" t="n">
         <v>7.01439197326757</v>
       </c>
-      <c r="U27" s="0" t="n">
-        <v>7.7505506343681</v>
-      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -1960,9 +1898,6 @@
       <c r="B28" s="0" t="n">
         <v>6.2635895666394</v>
       </c>
-      <c r="C28" s="0" t="n">
-        <v>4.85190037796158</v>
-      </c>
       <c r="D28" s="0" t="n">
         <v>6.47327749579116</v>
       </c>
@@ -2033,9 +1968,6 @@
       </c>
       <c r="E29" s="0" t="n">
         <v>6.32530080967461</v>
-      </c>
-      <c r="F29" s="0" t="n">
-        <v>4.61146148772846</v>
       </c>
       <c r="G29" s="0" t="n">
         <v>4.17034254487253</v>

</xml_diff>